<commit_message>
Updated PP, installed react-scripts for fitorfail, updated Completed Tasks
</commit_message>
<xml_diff>
--- a/Completed Tasks.xlsx
+++ b/Completed Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Task</t>
   </si>
@@ -572,7 +572,7 @@
   <dimension ref="B1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +635,9 @@
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -698,7 +700,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final PowerPoint, updated Completed Tasks, made wbs.png fully transparent
</commit_message>
<xml_diff>
--- a/Completed Tasks.xlsx
+++ b/Completed Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Task</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Gantt chart</t>
+  </si>
+  <si>
+    <t>Christian, Travis</t>
   </si>
 </sst>
 </file>
@@ -572,7 +575,7 @@
   <dimension ref="B1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,19 +646,25 @@
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">

</xml_diff>